<commit_message>
Edited Excel File C7-C19
</commit_message>
<xml_diff>
--- a/Datenerhebung.xlsx
+++ b/Datenerhebung.xlsx
@@ -14,9 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Beispieländerung</t>
+  </si>
+  <si>
+    <t>ldjf</t>
+  </si>
+  <si>
+    <t>kdjkdjf</t>
+  </si>
+  <si>
+    <t>dlff</t>
+  </si>
+  <si>
+    <t>ijdf</t>
   </si>
 </sst>
 </file>
@@ -358,17 +370,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>